<commit_message>
Add openpose frame numbers
</commit_message>
<xml_diff>
--- a/Unity_gesteIA/Assets/frames.xlsx
+++ b/Unity_gesteIA/Assets/frames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Info\Unity\GesteIA\Unity_gesteIA\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB24E38-AE06-4342-983F-7E9674DC8179}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173E7949-BD6C-4DC0-872B-4EBAF18CEAA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C79F11DA-EA4B-4CBD-BD86-FCDB15462959}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>25.19222</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>49.70855</t>
+  </si>
+  <si>
+    <t>Frame Openpose</t>
   </si>
 </sst>
 </file>
@@ -595,15 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D15354-A7E7-40DF-8D4C-BEE259C9C5C6}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -611,260 +614,276 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2">
         <v>1492</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <f>27*25</f>
+        <v>675</v>
+      </c>
+      <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
       <c r="B3">
         <v>2824</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>1243</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>24</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4">
         <v>1492</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>675</v>
+      </c>
+      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>45</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>47</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>48</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>49</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>50</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>51</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>52</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
       <c r="B5">
         <v>2824</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>1243</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>58</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>59</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>60</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>61</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>62</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>63</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>64</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>65</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>66</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>67</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>68</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>